<commit_message>
Tested and verified functionalities using sqlite
Signed-off-by: eaingaran <eaingaran@gmail.com>
</commit_message>
<xml_diff>
--- a/MasterConfig.xlsx
+++ b/MasterConfig.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Avinash\3G\Aingaran\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aingaran/PycharmProjects/virtual_env/TimeMachine/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="16380" windowHeight="8200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Database Type</t>
   </si>
@@ -67,28 +67,64 @@
     <t>Result Format</t>
   </si>
   <si>
-    <t>Test Scenario</t>
-  </si>
-  <si>
-    <t>Select 'Test' from dual</t>
-  </si>
-  <si>
-    <t>base_dir/test_folder/actual_file.csv</t>
-  </si>
-  <si>
-    <t>base_dir/test_folder/expected_file.csv</t>
-  </si>
-  <si>
-    <t>base_dir/test_folder/result_file.xlsx</t>
-  </si>
-  <si>
     <t>.xlsx</t>
+  </si>
+  <si>
+    <t>SQLite</t>
+  </si>
+  <si>
+    <t>local.db</t>
+  </si>
+  <si>
+    <t>.xlsm</t>
+  </si>
+  <si>
+    <t>Test XLSM Scenario</t>
+  </si>
+  <si>
+    <t>Test XLSX Scenario</t>
+  </si>
+  <si>
+    <t>Test HTML Scenario</t>
+  </si>
+  <si>
+    <t>.html</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_xlsm/expected_file.csv</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_xlsm/actual_file.csv</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_xlsx/actual_file.csv</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_xlsx/expected_file.csv</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_html/actual_file.csv</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_html/expected_file.csv</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_xlsm/result_file.xlsm</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_xlsx/result_file.xlsx</t>
+  </si>
+  <si>
+    <t>base_dir/test_folder_html/result_file.html</t>
+  </si>
+  <si>
+    <t>Select 'id;name' union select id||';'||name from user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -124,10 +160,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -497,19 +532,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.5703125" style="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,31 +561,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -567,23 +603,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -603,24 +639,64 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>